<commit_message>
bind "" to null
</commit_message>
<xml_diff>
--- a/2nrs-mtv8.xlsx
+++ b/2nrs-mtv8.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal\source\repos\xlladdins\xll_sqlite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBC8459-FB83-4ED5-998E-F024175C8680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BD8C83-CDEE-4618-BB23-9026D2492E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2715" yWindow="4635" windowWidth="28515" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="1350" windowWidth="30240" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2nrs-mtv8" sheetId="1" r:id="rId1"/>
     <sheet name="query" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -6279,9 +6278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB1001"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -6374,7 +6371,7 @@
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2">
         <f ca="1">RAND()</f>
-        <v>0.11974504185036317</v>
+        <v>0.56542868945173819</v>
       </c>
       <c r="B2" t="s">
         <v>28</v>
@@ -77096,9 +77093,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:L1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
@@ -77111,7 +77106,7 @@
       </c>
       <c r="C2" cm="1">
         <f t="array" ref="C2">_xll.\SQL.DB()</f>
-        <v>3124252745536</v>
+        <v>2711614899440</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
@@ -77120,7 +77115,7 @@
       </c>
       <c r="C3" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">_xll.SQL.CREATE_TABLE(C2, B3, '2nrs-mtv8'!A1:AB1001)</f>
-        <v>3124252745536</v>
+        <v>2711614899440</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
@@ -77167,7 +77162,7 @@
       </c>
       <c r="G6" t="str">
         <f ca="1"/>
-        <v>CREATE TABLE [2nrs-mtv8] (dr_no DOUBLE, date_rptd DATETIME, date_occ DATETIME, time_occ INTEGER, area INTEGER, area_name TEXT, rpt_dist_no INTEGER, part_1_2 INTEGER, crm_cd INTEGER, crm_cd_desc TEXT, mocodes TEXT, vict_age INTEGER, vict_sex TEXT, vict_descent TEXT, premis_cd INTEGER, premis_desc TEXT, weapon_used_cd INTEGER, weapon_desc TEXT, status TEXT, status_desc TEXT, crm_cd_1 INTEGER, crm_cd_2 INTEGER, crm_cd_3 TEXT, crm_cd_4 TEXT, location TEXT, cross_street TEXT, lat DOUBLE, lon DOUBLE)</v>
+        <v>CREATE TABLE [2nrs-mtv8] ([dr_no] DOUBLE, [date_rptd] DATETIME, [date_occ] DATETIME, [time_occ] INTEGER, [area] INTEGER, [area_name] TEXT, [rpt_dist_no] INTEGER, [part_1_2] INTEGER, [crm_cd] INTEGER, [crm_cd_desc] TEXT, [mocodes] TEXT, [vict_age] INTEGER, [vict_sex] TEXT, [vict_descent] TEXT, [premis_cd] INTEGER, [premis_desc] TEXT, [weapon_used_cd] INTEGER, [weapon_desc] TEXT, [status] TEXT, [status_desc] TEXT, [crm_cd_1] INTEGER, [crm_cd_2] INTEGER, [crm_cd_3] TEXT, [crm_cd_4] TEXT, [location] TEXT, [cross_street] TEXT, [lat] DOUBLE, [lon] DOUBLE)</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
@@ -77265,7 +77260,7 @@
       </c>
       <c r="J10" cm="1">
         <f t="array" aca="1" ref="J10:L1009" ca="1">_xlfn.DROP(_xll.SQL.QUERY(C3,J8),1)</f>
-        <v>0.11974504185036317</v>
+        <v>0.56542868945173819</v>
       </c>
       <c r="K10">
         <f ca="1"/>

</xml_diff>